<commit_message>
changes for reading file name from file name column
</commit_message>
<xml_diff>
--- a/public/images/admin/Master File for Codes and attributes - AJ - 26.04.22.xlsx
+++ b/public/images/admin/Master File for Codes and attributes - AJ - 26.04.22.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\personal\amit_repository\image gallery\prem_europa_provided\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC984364-816B-4B1E-864A-0B347640C375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="3180" windowWidth="20055" windowHeight="4770" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FABRICS" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -344,12 +350,57 @@
   <si>
     <t xml:space="preserve">Made from 100% Cotton. Normal / conventional Cotton and Organic Cotton. Size : Custom Made as per requirement. </t>
   </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>File name ending with 155140.jpg, 161327.jpg</t>
+  </si>
+  <si>
+    <t>dandelion black.jpg, dandelion blue.jpg, dandelion grey.jpg,  feather blue.jpg, feather grey.jpg and feather khaki.jpg</t>
+  </si>
+  <si>
+    <t>rabbit blue.jpg, rabbit grey.jpg</t>
+  </si>
+  <si>
+    <t>bear glasses.jpg, swan.jpg, flower.jpg, girl cloud.jpg, boy cloud parachute.jpg</t>
+  </si>
+  <si>
+    <t>horse ink.jpg, horse light blue.jpg, horse pink.jpg</t>
+  </si>
+  <si>
+    <t>Extra Jamna Plena.jpg, plena de-luxe 70x70.jpg, box packing.jpg</t>
+  </si>
+  <si>
+    <t>Fancy woven 1 cm Checks.jpeg, Fancy yarn dyed checks 1cm.jpg, Yarn dyed checks 0.5cm Red.jpg,yarn dyed checks 0.5cm.jpg</t>
+  </si>
+  <si>
+    <t>Plain white Satin.jpg</t>
+  </si>
+  <si>
+    <t>White Fabric with OB.jpg, White Fabric with OB02.jpg</t>
+  </si>
+  <si>
+    <t>ending with 160232.jpg, stripe satin 2.jpg, stripe satin 3.jpg, Satin 1cm Stripe 02.jpg, Satin 1cm Stripe.jpg, Satin 1cm Stripe 04.jpg, Satin Stripe 2 cm.jpg, Satin Stripe 2 cm-2.jpg.</t>
+  </si>
+  <si>
+    <t>Table cloths.jpg</t>
+  </si>
+  <si>
+    <t>Tea Towels 02.jpg, Tea Towels.jpg</t>
+  </si>
+  <si>
+    <t>Bed Set - 1.jpg, Bed Set - 2.jpg, Bed Set - 3.jpg, Bed Set - 4.jpg</t>
+  </si>
+  <si>
+    <t>5 mm Satin Checks Dobby.jpg, 5 mm Satin Checks dobby02.jpg, 5 mm Satin Checks Dobby03.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +630,14 @@
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -586,20 +645,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38103</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1067522</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>742950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3074" name="Picture 2"/>
+        <xdr:cNvPr id="3074" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000020C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -626,20 +691,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1181103</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>47627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2076450</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>710433</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3076" name="Picture 4"/>
+        <xdr:cNvPr id="3076" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000040C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -666,20 +737,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>66678</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>66678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1023786</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>781050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3078" name="Picture 6"/>
+        <xdr:cNvPr id="3078" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000060C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -706,20 +783,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1095377</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>76203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2019301</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>737288</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3080" name="Picture 8"/>
+        <xdr:cNvPr id="3080" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000080C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -746,20 +829,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2152651</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3303700</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>809625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3082" name="Picture 10"/>
+        <xdr:cNvPr id="3082" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A0C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -791,20 +880,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>209551</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>568080</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>571500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -831,20 +926,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>752477</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1476375</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>613378</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPr id="1028" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -871,20 +972,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1619251</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>104777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2266950</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>587295</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Picture 6"/>
+        <xdr:cNvPr id="1030" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -911,20 +1018,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2390777</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>625660</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1032" name="Picture 8"/>
+        <xdr:cNvPr id="1032" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -956,20 +1069,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>23154</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>685799</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>729135</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="Premium - dandelion black.jpg"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Premium - dandelion black.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -994,20 +1113,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1581151</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>581025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="Premium - dandelion blue.jpg"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Premium - dandelion blue.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1032,20 +1157,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1730204</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2238375</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>707962</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="Premium - dandelion grey.jpg"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Premium - dandelion grey.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1070,20 +1201,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2409825</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>9527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2962273</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>746355</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="Premium - feather blue.jpg"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="Premium - feather blue.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1108,20 +1245,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3102927</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3609975</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>704850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="Premium - feather grey.jpg"/>
+        <xdr:cNvPr id="12" name="Picture 11" descr="Premium - feather grey.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1146,20 +1289,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3810000</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>4505324</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>761310</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="Premium - feather khaki.jpg"/>
+        <xdr:cNvPr id="13" name="Picture 12" descr="Premium - feather khaki.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1184,20 +1333,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>48703</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>678433</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1224,20 +1379,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1000927</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>19052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1590675</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>733426</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPr id="1028" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1264,20 +1425,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>161926</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>858852</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>609600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Picture 6"/>
+        <xdr:cNvPr id="1030" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1304,20 +1471,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>996041</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>66677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1857375</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>714375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1032" name="Picture 8"/>
+        <xdr:cNvPr id="1032" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1344,20 +1517,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2038352</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2933700</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>735174</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1034" name="Picture 10"/>
+        <xdr:cNvPr id="1034" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1384,20 +1563,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3048001</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3961978</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>742950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1036" name="Picture 12"/>
+        <xdr:cNvPr id="1036" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1424,20 +1609,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>4114801</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>4989057</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>752475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1038" name="Picture 14"/>
+        <xdr:cNvPr id="1038" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1464,20 +1655,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>142876</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952926</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>704850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1040" name="Picture 16"/>
+        <xdr:cNvPr id="1040" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1504,20 +1701,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1162051</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2124075</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>781997</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1042" name="Picture 18"/>
+        <xdr:cNvPr id="1042" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1544,20 +1747,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>2333625</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3243506</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>752475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1044" name="Picture 20"/>
+        <xdr:cNvPr id="1044" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1589,20 +1798,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>98407</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>609605</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>717763</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPr id="2050" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1629,20 +1844,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>790577</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>76202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1192858</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>695326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPr id="2052" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1669,20 +1890,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1400177</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>57153</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1895475</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>738401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2054" name="Picture 6"/>
+        <xdr:cNvPr id="2054" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1753,7 +1980,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1785,9 +2012,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1819,6 +2064,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1994,26 +2257,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="51.7109375" customWidth="1"/>
+    <col min="4" max="5" width="59.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1"/>
+    <col min="7" max="7" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75">
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75">
+    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -2023,12 +2288,15 @@
       <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="2:7" ht="69.95" customHeight="1">
+    <row r="5" spans="2:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>35</v>
       </c>
@@ -2038,13 +2306,16 @@
       <c r="D5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="25"/>
       <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="2:7" ht="63.75">
+    <row r="6" spans="2:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>37</v>
       </c>
@@ -2054,13 +2325,16 @@
       <c r="D6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="25"/>
       <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="2:7" ht="47.25">
+    <row r="7" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>39</v>
       </c>
@@ -2070,13 +2344,16 @@
       <c r="D7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="25"/>
       <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="2:7" ht="47.25">
+    <row r="8" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>44</v>
       </c>
@@ -2086,13 +2363,16 @@
       <c r="D8" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="25"/>
       <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="2:7" ht="60" customHeight="1">
+    <row r="9" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>29</v>
       </c>
@@ -2102,13 +2382,16 @@
       <c r="D9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="25"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="2:7" ht="76.5">
+    <row r="10" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>32</v>
       </c>
@@ -2118,11 +2401,14 @@
       <c r="D10" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="25"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2132,26 +2418,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" customWidth="1"/>
+    <col min="4" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="7" max="7" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75">
+    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75">
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -2161,11 +2449,14 @@
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="38.25">
+    <row r="5" spans="2:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2175,11 +2466,14 @@
       <c r="D5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="51">
+    <row r="6" spans="2:7" ht="51" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>55</v>
       </c>
@@ -2189,11 +2483,14 @@
       <c r="D6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="60" customHeight="1">
+    <row r="7" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
         <v>59</v>
       </c>
@@ -2203,10 +2500,13 @@
       <c r="D7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2216,27 +2516,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" style="12" customWidth="1"/>
     <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
-    <col min="5" max="5" width="54.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="88.140625" customWidth="1"/>
+    <col min="4" max="5" width="54.7109375" customWidth="1"/>
+    <col min="6" max="6" width="54.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="88.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75">
+    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75">
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -2246,11 +2548,14 @@
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="63">
+    <row r="5" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
@@ -2260,12 +2565,15 @@
       <c r="D5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:6" ht="63">
+    <row r="6" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>12</v>
       </c>
@@ -2275,12 +2583,15 @@
       <c r="D6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:6" ht="63">
+    <row r="7" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
@@ -2290,12 +2601,15 @@
       <c r="D7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:6" ht="63">
+    <row r="8" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
@@ -2305,10 +2619,13 @@
       <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2318,21 +2635,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:G3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="4" max="5" width="52.140625" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75">
+    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2342,11 +2661,14 @@
       <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="60" customHeight="1">
+    <row r="3" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2356,10 +2678,13 @@
       <c r="D3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>